<commit_message>
save work on paper
</commit_message>
<xml_diff>
--- a/Data/Paper/GunshotTPRresults.xlsx
+++ b/Data/Paper/GunshotTPRresults.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21425"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60EC31EB-57CE-44EF-A9A3-B8830B8BE9DD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E28B2642-4A83-473F-95A2-A4BF382BE0D5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="1433" windowWidth="13546" windowHeight="11579" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12780" yWindow="1365" windowWidth="14685" windowHeight="11475" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -588,8 +588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24:D31"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>

</xml_diff>